<commit_message>
doc: Update Azure Costs spreadsheet with latest data
</commit_message>
<xml_diff>
--- a/docs/resources/Azure Costs.xlsx
+++ b/docs/resources/Azure Costs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Teragone\audit_cisac\docs\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BC4FA784-59B7-4D6F-A4AA-3057A97CF3C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D387D50-3A67-4FB8-BC61-06BC027F9CEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42510" yWindow="5715" windowWidth="20715" windowHeight="14880" xr2:uid="{760EA4E0-9FD1-497A-84FE-716C960294FC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{760EA4E0-9FD1-497A-84FE-716C960294FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>PROD</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>DEV</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
   </si>
 </sst>
 </file>
@@ -99,6 +102,1398 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR"/>
+              <a:t>Azure Costs</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="5.676088666476338E-2"/>
+          <c:y val="0.14164818289694411"/>
+          <c:w val="0.92688981126283643"/>
+          <c:h val="0.71000563411248985"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Feuil1!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>PROD</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Feuil1!$B$1:$N$1</c:f>
+              <c:numCache>
+                <c:formatCode>mmm\-yy</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>45931</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45901</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45870</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45839</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45809</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>45778</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="d\-mmm">
+                  <c:v>45748</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45717</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45689</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45658</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>45627</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>45597</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>45566</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Feuil1!$B$2:$N$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>28089</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>27937</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27448</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>26073</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>26088</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>27625</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30740</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>29820</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>34242</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>29690</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>23550</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>20182</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>23323</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-EE52-4E87-A1FC-E04410934D54}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Feuil1!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>UAT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Feuil1!$B$1:$N$1</c:f>
+              <c:numCache>
+                <c:formatCode>mmm\-yy</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>45931</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45901</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45870</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45839</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45809</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>45778</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="d\-mmm">
+                  <c:v>45748</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45717</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45689</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45658</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>45627</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>45597</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>45566</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Feuil1!$B$3:$N$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>2655</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2669</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2831</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2725</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3191</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2782</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2975</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3160</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2463</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3039</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4194</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2363</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2482</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-EE52-4E87-A1FC-E04410934D54}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Feuil1!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>DEV</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Feuil1!$B$1:$N$1</c:f>
+              <c:numCache>
+                <c:formatCode>mmm\-yy</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>45931</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45901</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45870</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45839</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45809</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>45778</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="d\-mmm">
+                  <c:v>45748</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45717</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45689</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45658</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>45627</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>45597</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>45566</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Feuil1!$B$4:$N$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1268</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1463</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1511</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1488</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1528</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1442</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1603</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1911</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1508</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1245</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1118</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1121</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1194</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-EE52-4E87-A1FC-E04410934D54}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Feuil1!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>TOTAL</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Feuil1!$B$1:$N$1</c:f>
+              <c:numCache>
+                <c:formatCode>mmm\-yy</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>45931</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45901</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45870</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45839</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45809</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>45778</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="d\-mmm">
+                  <c:v>45748</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45717</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45689</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45658</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>45627</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>45597</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>45566</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Feuil1!$B$5:$N$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>32012</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32069</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>31790</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30286</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30807</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>31849</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35318</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>34891</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>38213</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>33974</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>28862</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>23666</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>26999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-EE52-4E87-A1FC-E04410934D54}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="698375231"/>
+        <c:axId val="698375711"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="698375231"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="mmm\-yy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="698375711"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="months"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="698375711"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="698375231"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>114299</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Graphique 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61D4B66D-5EC7-BEFA-A500-93BCED61708C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -421,7 +1816,7 @@
   <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,6 +2007,9 @@
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
       <c r="B5">
         <f>SUM(B2:B4)</f>
         <v>32012</v>
@@ -672,5 +2070,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
doc: Update Azure Costs spreadsheet with new data
</commit_message>
<xml_diff>
--- a/docs/resources/Azure Costs.xlsx
+++ b/docs/resources/Azure Costs.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Teragone\audit_cisac\docs\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D387D50-3A67-4FB8-BC61-06BC027F9CEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA3E5B9A-820E-4455-8997-90C3596A5FEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{760EA4E0-9FD1-497A-84FE-716C960294FC}"/>
+    <workbookView xWindow="4125" yWindow="4170" windowWidth="30225" windowHeight="15990" xr2:uid="{760EA4E0-9FD1-497A-84FE-716C960294FC}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Total" sheetId="1" r:id="rId1"/>
+    <sheet name="Itemized" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>PROD</t>
   </si>
@@ -49,11 +50,80 @@
   <si>
     <t>TOTAL</t>
   </si>
+  <si>
+    <t>SQL</t>
+  </si>
+  <si>
+    <t>Databrick</t>
+  </si>
+  <si>
+    <t>API Management</t>
+  </si>
+  <si>
+    <t>Bandwith</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>App Service</t>
+  </si>
+  <si>
+    <t>CosmoDb</t>
+  </si>
+  <si>
+    <t>Moyenne</t>
+  </si>
+  <si>
+    <t>Colonne1</t>
+  </si>
+  <si>
+    <t>oct-25</t>
+  </si>
+  <si>
+    <t>sept-25</t>
+  </si>
+  <si>
+    <t>août-25</t>
+  </si>
+  <si>
+    <t>juil-25</t>
+  </si>
+  <si>
+    <t>juin-25</t>
+  </si>
+  <si>
+    <t>mai-25</t>
+  </si>
+  <si>
+    <t>01-avr</t>
+  </si>
+  <si>
+    <t>mars-25</t>
+  </si>
+  <si>
+    <t>févr-25</t>
+  </si>
+  <si>
+    <t>janv-25</t>
+  </si>
+  <si>
+    <t>déc-24</t>
+  </si>
+  <si>
+    <t>nov-24</t>
+  </si>
+  <si>
+    <t>oct-24</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;€&quot;"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -83,15 +153,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <numFmt numFmtId="22" formatCode="mmm\-yy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -194,7 +272,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Feuil1!$A$2</c:f>
+              <c:f>Total!$A$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -217,7 +295,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Feuil1!$B$1:$N$1</c:f>
+              <c:f>Total!$B$1:$N$1</c:f>
               <c:numCache>
                 <c:formatCode>mmm\-yy</c:formatCode>
                 <c:ptCount val="13"/>
@@ -265,7 +343,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$B$2:$N$2</c:f>
+              <c:f>Total!$B$2:$N$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -323,7 +401,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Feuil1!$A$3</c:f>
+              <c:f>Total!$A$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -346,7 +424,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Feuil1!$B$1:$N$1</c:f>
+              <c:f>Total!$B$1:$N$1</c:f>
               <c:numCache>
                 <c:formatCode>mmm\-yy</c:formatCode>
                 <c:ptCount val="13"/>
@@ -394,7 +472,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$B$3:$N$3</c:f>
+              <c:f>Total!$B$3:$N$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -452,7 +530,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Feuil1!$A$4</c:f>
+              <c:f>Total!$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -475,7 +553,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Feuil1!$B$1:$N$1</c:f>
+              <c:f>Total!$B$1:$N$1</c:f>
               <c:numCache>
                 <c:formatCode>mmm\-yy</c:formatCode>
                 <c:ptCount val="13"/>
@@ -523,7 +601,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$B$4:$N$4</c:f>
+              <c:f>Total!$B$4:$N$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -581,7 +659,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Feuil1!$A$5</c:f>
+              <c:f>Total!$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -604,7 +682,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Feuil1!$B$1:$N$1</c:f>
+              <c:f>Total!$B$1:$N$1</c:f>
               <c:numCache>
                 <c:formatCode>mmm\-yy</c:formatCode>
                 <c:ptCount val="13"/>
@@ -652,9 +730,9 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$B$5:$N$5</c:f>
+              <c:f>Total!$B$5:$N$5</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>#\ ##0.00\ "€"</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>32012</c:v>
@@ -899,7 +977,1057 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Itemized!$A$2:$H$2</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>CosmoDb</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15105</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16296</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14799</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Itemized!$I$1:$O$1</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Itemized!$I$1:$N$1</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>mars-25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>févr-25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>janv-25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>déc-24</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>nov-24</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>oct-24</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Itemized!$I$2:$O$2</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Itemized!$I$2:$N$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>16161</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24135</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18829</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12909</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11329</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13483</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8719-43AE-8944-FD24C6EB7E86}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Itemized!$A$3:$H$3</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>SQL</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4435</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4515</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4647</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Itemized!$I$1:$O$1</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Itemized!$I$1:$N$1</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>mars-25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>févr-25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>janv-25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>déc-24</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>nov-24</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>oct-24</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Itemized!$I$3:$O$3</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Itemized!$I$3:$N$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>4614</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4487</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4971</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4915</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4624</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4620</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8719-43AE-8944-FD24C6EB7E86}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Itemized!$A$4:$H$4</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Databrick</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3897</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4057</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7734</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Itemized!$I$1:$O$1</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Itemized!$I$1:$N$1</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>mars-25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>févr-25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>janv-25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>déc-24</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>nov-24</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>oct-24</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Itemized!$I$4:$O$4</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Itemized!$I$4:$N$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>4614</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2375</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2596</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2441</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1296</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2192</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-8719-43AE-8944-FD24C6EB7E86}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Itemized!$A$5:$H$5</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>API Management</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1198</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1230</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1254</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Itemized!$I$1:$O$1</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Itemized!$I$1:$N$1</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>mars-25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>févr-25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>janv-25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>déc-24</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>nov-24</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>oct-24</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Itemized!$I$5:$O$5</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Itemized!$I$5:$N$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1332</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1213</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1343</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1335</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1254</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1253</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-8719-43AE-8944-FD24C6EB7E86}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Itemized!$A$6:$H$6</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>App Service</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1089</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>996</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1208</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Itemized!$I$1:$O$1</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Itemized!$I$1:$N$1</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>mars-25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>févr-25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>janv-25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>déc-24</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>nov-24</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>oct-24</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Itemized!$I$6:$O$6</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Itemized!$I$6:$N$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1306</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1172</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1273</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1281</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1102</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1156</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-8719-43AE-8944-FD24C6EB7E86}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Itemized!$A$7:$H$7</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Bandwith</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2,86</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2,74</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2,58</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Itemized!$I$1:$O$1</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Itemized!$I$1:$N$1</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>mars-25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>févr-25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>janv-25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>déc-24</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>nov-24</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>oct-24</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Itemized!$I$7:$O$7</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Itemized!$I$7:$N$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.61</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.69</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.85</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.77</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.72</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-8719-43AE-8944-FD24C6EB7E86}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Itemized!$A$8:$H$8</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25 726,86 €</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>27 096,74 €</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>29 644,58 €</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Itemized!$I$1:$O$1</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Itemized!$I$1:$N$1</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>mars-25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>févr-25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>janv-25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>déc-24</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>nov-24</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>oct-24</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Itemized!$I$8:$O$8</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Itemized!$I$8:$N$8</c:f>
+              <c:numCache>
+                <c:formatCode>#\ ##0.00\ "€"</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>28034</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>33385.61</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>29015.69</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22888.85</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>19607.77</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22708.720000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-8719-43AE-8944-FD24C6EB7E86}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="936731471"/>
+        <c:axId val="936732431"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="936731471"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="936732431"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="936732431"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="936731471"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1455,20 +2583,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>114299</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>66674</xdr:rowOff>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>76199</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>180976</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1494,6 +3138,132 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graphique 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D589BECD-5038-9C1F-A6AE-7AB927218C34}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Image 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{473F0929-8EBC-8941-037A-8ADDB037A263}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9477375" y="2771775"/>
+          <a:ext cx="12172950" cy="1790700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C5C38419-F688-4753-9DC0-E5CFC32CBB6D}" name="Tableau1" displayName="Tableau1" ref="A1:O8" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:O8" xr:uid="{C5C38419-F688-4753-9DC0-E5CFC32CBB6D}"/>
+  <tableColumns count="15">
+    <tableColumn id="1" xr3:uid="{963C741E-FBC1-4DFE-94D3-47CE7B5F2A1A}" name="Colonne1"/>
+    <tableColumn id="2" xr3:uid="{5B9820A2-FBBB-4706-B250-AFB9F6F1E542}" name="oct-25"/>
+    <tableColumn id="3" xr3:uid="{EFA2D109-D75E-4B93-8CB5-734672B13A75}" name="sept-25"/>
+    <tableColumn id="4" xr3:uid="{279ADEE5-C271-4FCD-A967-A572C4831A6F}" name="août-25"/>
+    <tableColumn id="5" xr3:uid="{046AACD6-7B47-48AE-B25B-F4894FCA06BE}" name="juil-25"/>
+    <tableColumn id="6" xr3:uid="{7483C9A9-3FBB-4686-B686-879DFEDD9CCF}" name="juin-25"/>
+    <tableColumn id="7" xr3:uid="{31BA766A-AB9B-4C86-B486-8FC614595B53}" name="mai-25"/>
+    <tableColumn id="8" xr3:uid="{7DDC1234-82FC-4C40-8BFC-8AB5543DAC6E}" name="01-avr"/>
+    <tableColumn id="9" xr3:uid="{FBD4B820-01D8-4CD0-8F13-A7F08C75E883}" name="mars-25"/>
+    <tableColumn id="10" xr3:uid="{DA4B76DE-422A-4EEC-A722-B6AB2CA9F6F8}" name="févr-25"/>
+    <tableColumn id="11" xr3:uid="{82B0AC29-E6F5-4F7E-B674-41F1781EE840}" name="janv-25"/>
+    <tableColumn id="12" xr3:uid="{60EFE477-3848-4D20-8B3E-6B658F62C54A}" name="déc-24"/>
+    <tableColumn id="13" xr3:uid="{300D5EB7-3725-4EDE-91B0-B9DD10BDA9B3}" name="nov-24"/>
+    <tableColumn id="14" xr3:uid="{ADB2C3F2-2F00-4C55-A6A8-BA4B19C08BDC}" name="oct-24"/>
+    <tableColumn id="15" xr3:uid="{629DAAA1-365A-4081-8BD0-3B225DA9302C}" name="Moyenne" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1816,7 +3586,7 @@
   <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1861,6 +3631,9 @@
       <c r="N1" s="1">
         <v>45566</v>
       </c>
+      <c r="O1" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1905,7 +3678,7 @@
       <c r="N2">
         <v>23323</v>
       </c>
-      <c r="O2">
+      <c r="O2" s="3">
         <f>AVERAGE(B2:N2)</f>
         <v>27292.846153846152</v>
       </c>
@@ -1953,7 +3726,7 @@
       <c r="N3">
         <v>2482</v>
       </c>
-      <c r="O3">
+      <c r="O3" s="3">
         <f>AVERAGE(B3:N3)</f>
         <v>2886.8461538461538</v>
       </c>
@@ -2001,68 +3774,68 @@
       <c r="N4">
         <v>1194</v>
       </c>
-      <c r="O4">
+      <c r="O4" s="3">
         <f>AVERAGE(B4:N4)</f>
         <v>1415.3846153846155</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="3">
         <f>SUM(B2:B4)</f>
         <v>32012</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="3">
         <f t="shared" ref="C5:O5" si="0">SUM(C2:C4)</f>
         <v>32069</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="3">
         <f t="shared" si="0"/>
         <v>31790</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="3">
         <f t="shared" si="0"/>
         <v>30286</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="3">
         <f t="shared" si="0"/>
         <v>30807</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="3">
         <f t="shared" si="0"/>
         <v>31849</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="3">
         <f t="shared" si="0"/>
         <v>35318</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="3">
         <f t="shared" si="0"/>
         <v>34891</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="3">
         <f t="shared" si="0"/>
         <v>38213</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="3">
         <f t="shared" si="0"/>
         <v>33974</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="3">
         <f t="shared" si="0"/>
         <v>28862</v>
       </c>
-      <c r="M5">
+      <c r="M5" s="3">
         <f t="shared" si="0"/>
         <v>23666</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="3">
         <f t="shared" si="0"/>
         <v>26999</v>
       </c>
-      <c r="O5">
+      <c r="O5" s="3">
         <f t="shared" si="0"/>
         <v>31595.076923076922</v>
       </c>
@@ -2072,4 +3845,427 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDE4E890-3AF0-487C-80B8-6CD4D7EA7705}">
+  <dimension ref="A1:Q12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2">
+        <v>15105</v>
+      </c>
+      <c r="G2">
+        <v>16296</v>
+      </c>
+      <c r="H2">
+        <v>14799</v>
+      </c>
+      <c r="I2">
+        <v>16161</v>
+      </c>
+      <c r="J2">
+        <v>24135</v>
+      </c>
+      <c r="K2">
+        <v>18829</v>
+      </c>
+      <c r="L2">
+        <v>12909</v>
+      </c>
+      <c r="M2">
+        <v>11329</v>
+      </c>
+      <c r="N2">
+        <v>13483</v>
+      </c>
+      <c r="O2" s="3">
+        <f>AVERAGE(I2:N2)</f>
+        <v>16141</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3">
+        <v>4435</v>
+      </c>
+      <c r="G3">
+        <v>4515</v>
+      </c>
+      <c r="H3">
+        <v>4647</v>
+      </c>
+      <c r="I3">
+        <v>4614</v>
+      </c>
+      <c r="J3">
+        <v>4487</v>
+      </c>
+      <c r="K3">
+        <v>4971</v>
+      </c>
+      <c r="L3">
+        <v>4915</v>
+      </c>
+      <c r="M3">
+        <v>4624</v>
+      </c>
+      <c r="N3">
+        <v>4620</v>
+      </c>
+      <c r="O3" s="3">
+        <f>AVERAGE(I3:N3)</f>
+        <v>4705.166666666667</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4">
+        <v>3897</v>
+      </c>
+      <c r="G4">
+        <v>4057</v>
+      </c>
+      <c r="H4">
+        <v>7734</v>
+      </c>
+      <c r="I4">
+        <v>4614</v>
+      </c>
+      <c r="J4">
+        <v>2375</v>
+      </c>
+      <c r="K4">
+        <v>2596</v>
+      </c>
+      <c r="L4">
+        <v>2441</v>
+      </c>
+      <c r="M4">
+        <v>1296</v>
+      </c>
+      <c r="N4">
+        <v>2192</v>
+      </c>
+      <c r="O4" s="3">
+        <f>AVERAGE(I4:N4)</f>
+        <v>2585.6666666666665</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5">
+        <v>1198</v>
+      </c>
+      <c r="G5">
+        <v>1230</v>
+      </c>
+      <c r="H5">
+        <v>1254</v>
+      </c>
+      <c r="I5">
+        <v>1332</v>
+      </c>
+      <c r="J5">
+        <v>1213</v>
+      </c>
+      <c r="K5">
+        <v>1343</v>
+      </c>
+      <c r="L5">
+        <v>1335</v>
+      </c>
+      <c r="M5">
+        <v>1254</v>
+      </c>
+      <c r="N5">
+        <v>1253</v>
+      </c>
+      <c r="O5" s="3">
+        <f>AVERAGE(I5:N5)</f>
+        <v>1288.3333333333333</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6">
+        <v>1089</v>
+      </c>
+      <c r="G6">
+        <v>996</v>
+      </c>
+      <c r="H6">
+        <v>1208</v>
+      </c>
+      <c r="I6">
+        <v>1306</v>
+      </c>
+      <c r="J6">
+        <v>1172</v>
+      </c>
+      <c r="K6">
+        <v>1273</v>
+      </c>
+      <c r="L6">
+        <v>1281</v>
+      </c>
+      <c r="M6">
+        <v>1102</v>
+      </c>
+      <c r="N6">
+        <v>1156</v>
+      </c>
+      <c r="O6" s="3">
+        <f>AVERAGE(I6:N6)</f>
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7">
+        <v>2.86</v>
+      </c>
+      <c r="G7">
+        <v>2.74</v>
+      </c>
+      <c r="H7">
+        <v>2.58</v>
+      </c>
+      <c r="I7">
+        <v>7</v>
+      </c>
+      <c r="J7">
+        <v>3.61</v>
+      </c>
+      <c r="K7">
+        <v>3.69</v>
+      </c>
+      <c r="L7">
+        <v>7.85</v>
+      </c>
+      <c r="M7">
+        <v>2.77</v>
+      </c>
+      <c r="N7">
+        <v>4.72</v>
+      </c>
+      <c r="O7" s="3">
+        <f>AVERAGE(I7:N7)</f>
+        <v>4.9399999999999995</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="3">
+        <f>SUM(F2:F7)</f>
+        <v>25726.86</v>
+      </c>
+      <c r="G8" s="3">
+        <f>SUM(G2:G7)</f>
+        <v>27096.74</v>
+      </c>
+      <c r="H8" s="3">
+        <f>SUM(H2:H7)</f>
+        <v>29644.58</v>
+      </c>
+      <c r="I8" s="3">
+        <f>SUM(I2:I7)</f>
+        <v>28034</v>
+      </c>
+      <c r="J8" s="3">
+        <f t="shared" ref="J8:O8" si="0">SUM(J2:J7)</f>
+        <v>33385.61</v>
+      </c>
+      <c r="K8" s="3">
+        <f t="shared" si="0"/>
+        <v>29015.69</v>
+      </c>
+      <c r="L8" s="3">
+        <f t="shared" si="0"/>
+        <v>22888.85</v>
+      </c>
+      <c r="M8" s="3">
+        <f t="shared" si="0"/>
+        <v>19607.77</v>
+      </c>
+      <c r="N8" s="3">
+        <f t="shared" si="0"/>
+        <v>22708.720000000001</v>
+      </c>
+      <c r="O8" s="3">
+        <f>SUM(I8:N8)</f>
+        <v>155640.63999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P12" s="2">
+        <v>45681</v>
+      </c>
+      <c r="Q12" s="2">
+        <v>45730</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="F2:N2">
+    <cfRule type="dataBar" priority="3">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{AA15D0CC-5405-47F5-BBC1-C66ED35E78EC}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F7:N7">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFB628"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{A8F5EA75-AEB1-4872-B806-1F62592B6942}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F8:N8">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{294FA6CB-5D9B-4E10-B098-7596CC80F18E}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{AA15D0CC-5405-47F5-BBC1-C66ED35E78EC}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>F2:N2</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{A8F5EA75-AEB1-4872-B806-1F62592B6942}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFFFB628"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>F7:N7</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{294FA6CB-5D9B-4E10-B098-7596CC80F18E}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFFF555A"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>F8:N8</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Correction Typo Smart AIM
</commit_message>
<xml_diff>
--- a/docs/resources/Azure Costs.xlsx
+++ b/docs/resources/Azure Costs.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Teragone\audit_cisac\docs\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA3E5B9A-820E-4455-8997-90C3596A5FEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E586BEC0-7F10-46C6-B13B-B36500333FA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4125" yWindow="4170" windowWidth="30225" windowHeight="15990" xr2:uid="{760EA4E0-9FD1-497A-84FE-716C960294FC}"/>
+    <workbookView xWindow="2130" yWindow="3675" windowWidth="30225" windowHeight="15990" xr2:uid="{760EA4E0-9FD1-497A-84FE-716C960294FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Total" sheetId="1" r:id="rId1"/>
     <sheet name="Itemized" sheetId="2" r:id="rId2"/>
+    <sheet name="Week" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="41">
   <si>
     <t>PROD</t>
   </si>
@@ -116,13 +117,58 @@
   <si>
     <t>oct-24</t>
   </si>
+  <si>
+    <t>Cosmo</t>
+  </si>
+  <si>
+    <t>13-19</t>
+  </si>
+  <si>
+    <t>27/1-2/2</t>
+  </si>
+  <si>
+    <t>3/2-9/2</t>
+  </si>
+  <si>
+    <t>10/3-16/2</t>
+  </si>
+  <si>
+    <t>17-2/23-2</t>
+  </si>
+  <si>
+    <t>24/2-2-/3</t>
+  </si>
+  <si>
+    <t>3/3-9/3</t>
+  </si>
+  <si>
+    <t>10/3-16/3</t>
+  </si>
+  <si>
+    <t>17/3-23/3</t>
+  </si>
+  <si>
+    <t>24/3-30-3</t>
+  </si>
+  <si>
+    <t>20-26</t>
+  </si>
+  <si>
+    <t>Somme</t>
+  </si>
+  <si>
+    <t>Résultat cumulé</t>
+  </si>
+  <si>
+    <t>Nombre</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;€&quot;"/>
+    <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -157,17 +203,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
-      <numFmt numFmtId="22" formatCode="mmm\-yy"/>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;€&quot;"/>
+      <numFmt numFmtId="22" formatCode="mmm\-yy"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1987,6 +2033,479 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Week!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cosmo</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Week!$B$1:$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>13-19</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20-26</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27/1-2/2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3/2-9/2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10/3-16/2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>17-2/23-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24/2-2-/3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3/3-9/3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10/3-16/3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>17/3-23/3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>24/3-30-3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Week!$B$2:$L$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>3450</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6093</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5923</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5390</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6848</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6643</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5072</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4075</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3023</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4486</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D05A-4AB7-A0F1-D347F81F1071}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Week!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Week!$B$1:$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>13-19</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20-26</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27/1-2/2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3/2-9/2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10/3-16/2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>17-2/23-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24/2-2-/3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3/3-9/3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10/3-16/3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>17/3-23/3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>24/3-30-3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Week!$B$3:$L$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>5900</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8629</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8470</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7837</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9284</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9041</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7919</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6759</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5741</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8027</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6793</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D05A-4AB7-A0F1-D347F81F1071}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="850196608"/>
+        <c:axId val="850203808"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="850196608"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="850203808"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="850203808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="850196608"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2067,6 +2586,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -2746,6 +3305,509 @@
       <a:solidFill>
         <a:schemeClr val="phClr"/>
       </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3242,8 +4304,110 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7CE4243E-F55F-4A8E-9E20-BEB0A301F136}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="38100" y="3429000"/>
+          <a:ext cx="12172950" cy="1790700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>33337</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>33337</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Graphique 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D2E17CD-8F51-859B-0B2A-9E643829C04F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C5C38419-F688-4753-9DC0-E5CFC32CBB6D}" name="Tableau1" displayName="Tableau1" ref="A1:O8" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C5C38419-F688-4753-9DC0-E5CFC32CBB6D}" name="Tableau1" displayName="Tableau1" ref="A1:O8" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="A1:O8" xr:uid="{C5C38419-F688-4753-9DC0-E5CFC32CBB6D}"/>
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{963C741E-FBC1-4DFE-94D3-47CE7B5F2A1A}" name="Colonne1"/>
@@ -3260,7 +4424,7 @@
     <tableColumn id="12" xr3:uid="{60EFE477-3848-4D20-8B3E-6B658F62C54A}" name="déc-24"/>
     <tableColumn id="13" xr3:uid="{300D5EB7-3725-4EDE-91B0-B9DD10BDA9B3}" name="nov-24"/>
     <tableColumn id="14" xr3:uid="{ADB2C3F2-2F00-4C55-A6A8-BA4B19C08BDC}" name="oct-24"/>
-    <tableColumn id="15" xr3:uid="{629DAAA1-365A-4081-8BD0-3B225DA9302C}" name="Moyenne" dataDxfId="1"/>
+    <tableColumn id="15" xr3:uid="{629DAAA1-365A-4081-8BD0-3B225DA9302C}" name="Moyenne" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3936,7 +5100,7 @@
         <v>13483</v>
       </c>
       <c r="O2" s="3">
-        <f>AVERAGE(I2:N2)</f>
+        <f t="shared" ref="O2:O7" si="0">AVERAGE(I2:N2)</f>
         <v>16141</v>
       </c>
     </row>
@@ -3972,7 +5136,7 @@
         <v>4620</v>
       </c>
       <c r="O3" s="3">
-        <f>AVERAGE(I3:N3)</f>
+        <f t="shared" si="0"/>
         <v>4705.166666666667</v>
       </c>
     </row>
@@ -4008,7 +5172,7 @@
         <v>2192</v>
       </c>
       <c r="O4" s="3">
-        <f>AVERAGE(I4:N4)</f>
+        <f t="shared" si="0"/>
         <v>2585.6666666666665</v>
       </c>
     </row>
@@ -4044,7 +5208,7 @@
         <v>1253</v>
       </c>
       <c r="O5" s="3">
-        <f>AVERAGE(I5:N5)</f>
+        <f t="shared" si="0"/>
         <v>1288.3333333333333</v>
       </c>
     </row>
@@ -4080,7 +5244,7 @@
         <v>1156</v>
       </c>
       <c r="O6" s="3">
-        <f>AVERAGE(I6:N6)</f>
+        <f t="shared" si="0"/>
         <v>1215</v>
       </c>
     </row>
@@ -4116,7 +5280,7 @@
         <v>4.72</v>
       </c>
       <c r="O7" s="3">
-        <f>AVERAGE(I7:N7)</f>
+        <f t="shared" si="0"/>
         <v>4.9399999999999995</v>
       </c>
     </row>
@@ -4141,23 +5305,23 @@
         <v>28034</v>
       </c>
       <c r="J8" s="3">
-        <f t="shared" ref="J8:O8" si="0">SUM(J2:J7)</f>
+        <f t="shared" ref="J8:N8" si="1">SUM(J2:J7)</f>
         <v>33385.61</v>
       </c>
       <c r="K8" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>29015.69</v>
       </c>
       <c r="L8" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>22888.85</v>
       </c>
       <c r="M8" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>19607.77</v>
       </c>
       <c r="N8" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>22708.720000000001</v>
       </c>
       <c r="O8" s="3">
@@ -4268,4 +5432,131 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DA97498-BE33-47CD-AFCE-24A11E184539}">
+  <dimension ref="A1:L3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:L3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2">
+        <v>3450</v>
+      </c>
+      <c r="C2">
+        <v>6093</v>
+      </c>
+      <c r="D2">
+        <v>5923</v>
+      </c>
+      <c r="E2">
+        <v>5390</v>
+      </c>
+      <c r="F2">
+        <v>6848</v>
+      </c>
+      <c r="G2">
+        <v>6643</v>
+      </c>
+      <c r="H2">
+        <v>5072</v>
+      </c>
+      <c r="I2">
+        <v>4075</v>
+      </c>
+      <c r="J2">
+        <v>3023</v>
+      </c>
+      <c r="K2">
+        <v>4486</v>
+      </c>
+      <c r="L2">
+        <v>3256</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>5900</v>
+      </c>
+      <c r="C3">
+        <v>8629</v>
+      </c>
+      <c r="D3">
+        <v>8470</v>
+      </c>
+      <c r="E3">
+        <v>7837</v>
+      </c>
+      <c r="F3">
+        <v>9284</v>
+      </c>
+      <c r="G3">
+        <v>9041</v>
+      </c>
+      <c r="H3">
+        <v>7919</v>
+      </c>
+      <c r="I3">
+        <v>6759</v>
+      </c>
+      <c r="J3">
+        <v>5741</v>
+      </c>
+      <c r="K3">
+        <v>8027</v>
+      </c>
+      <c r="L3">
+        <v>6793</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>